<commit_message>
Fig 3 update-mpa export
</commit_message>
<xml_diff>
--- a/outputs/tables/Clustering.xlsx
+++ b/outputs/tables/Clustering.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Carreira Acadêmica/Doutorado/Tese - João Paulo Alencar/Analises/Elementos Bióticos/Resultados/BE_Cerrado/outputs/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A7ABE7-6B6F-2F4D-BBAF-8A92257C79DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCECD6F5-8D60-BA49-97A8-BAD6957BDCAE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5900" yWindow="-14400" windowWidth="25600" windowHeight="14360" activeTab="5" xr2:uid="{8BE1F850-643F-754B-B438-8BDD7E09D5AB}"/>
+    <workbookView xWindow="2600" yWindow="-18820" windowWidth="25600" windowHeight="14360" activeTab="3" xr2:uid="{8BE1F850-643F-754B-B438-8BDD7E09D5AB}"/>
   </bookViews>
   <sheets>
     <sheet name="cdn" sheetId="2" r:id="rId1"/>
@@ -1967,6 +1967,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1985,7 +1986,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2356,7 +2356,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="117" t="s">
+      <c r="A3" s="118" t="s">
         <v>329</v>
       </c>
       <c r="B3" t="s">
@@ -2391,7 +2391,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="117"/>
+      <c r="A4" s="118"/>
       <c r="B4" t="s">
         <v>352</v>
       </c>
@@ -2424,7 +2424,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="117"/>
+      <c r="A5" s="118"/>
       <c r="B5" t="s">
         <v>351</v>
       </c>
@@ -2457,7 +2457,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="117" t="s">
+      <c r="A7" s="118" t="s">
         <v>330</v>
       </c>
       <c r="B7" t="s">
@@ -2492,7 +2492,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="117"/>
+      <c r="A8" s="118"/>
       <c r="B8" t="s">
         <v>352</v>
       </c>
@@ -2525,7 +2525,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="117"/>
+      <c r="A9" s="118"/>
       <c r="B9" t="s">
         <v>351</v>
       </c>
@@ -2558,7 +2558,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="117" t="s">
+      <c r="A11" s="118" t="s">
         <v>331</v>
       </c>
       <c r="B11" t="s">
@@ -2593,7 +2593,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="117"/>
+      <c r="A12" s="118"/>
       <c r="B12" t="s">
         <v>352</v>
       </c>
@@ -2626,7 +2626,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="117"/>
+      <c r="A13" s="118"/>
       <c r="B13" t="s">
         <v>351</v>
       </c>
@@ -2659,7 +2659,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="117" t="s">
+      <c r="A15" s="118" t="s">
         <v>332</v>
       </c>
       <c r="B15" t="s">
@@ -2694,7 +2694,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="117"/>
+      <c r="A16" s="118"/>
       <c r="B16" t="s">
         <v>352</v>
       </c>
@@ -2727,7 +2727,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="117"/>
+      <c r="A17" s="118"/>
       <c r="B17" t="s">
         <v>351</v>
       </c>
@@ -2760,7 +2760,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="118" t="s">
+      <c r="A19" s="119" t="s">
         <v>333</v>
       </c>
       <c r="B19" s="7" t="s">
@@ -2795,7 +2795,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="118"/>
+      <c r="A20" s="119"/>
       <c r="B20" s="7" t="s">
         <v>352</v>
       </c>
@@ -2828,7 +2828,7 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="119"/>
+      <c r="A21" s="120"/>
       <c r="B21" s="8" t="s">
         <v>351</v>
       </c>
@@ -2900,15 +2900,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="121" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="120"/>
+      <c r="B1" s="121"/>
       <c r="C1" s="25"/>
-      <c r="D1" s="120" t="s">
+      <c r="D1" s="121" t="s">
         <v>305</v>
       </c>
-      <c r="E1" s="120"/>
+      <c r="E1" s="121"/>
       <c r="G1" s="26" t="s">
         <v>385</v>
       </c>
@@ -14951,9 +14951,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48956B19-CF25-1042-B320-1547212FD114}">
   <dimension ref="A1:Q37"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G18" activeCellId="1" sqref="G2:G13 G18:G30"/>
+      <selection pane="bottomLeft" activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15016,47 +15016,47 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2" s="12">
-        <v>6</v>
+      <c r="A2" s="12" t="s">
+        <v>447</v>
       </c>
       <c r="B2" s="103">
-        <v>7</v>
-      </c>
-      <c r="C2" s="67">
+        <v>4</v>
+      </c>
+      <c r="C2" s="21">
+        <v>1</v>
+      </c>
+      <c r="D2" s="21">
+        <v>0</v>
+      </c>
+      <c r="E2" s="21">
+        <v>0</v>
+      </c>
+      <c r="F2" s="21">
+        <v>2</v>
+      </c>
+      <c r="G2" s="21">
+        <v>1</v>
+      </c>
+      <c r="H2" s="16">
         <v>3</v>
       </c>
-      <c r="D2" s="67">
-        <v>2</v>
-      </c>
-      <c r="E2" s="67">
+      <c r="I2" s="91">
+        <v>216523</v>
+      </c>
+      <c r="J2" s="12">
+        <v>18</v>
+      </c>
+      <c r="K2" s="12">
+        <v>0</v>
+      </c>
+      <c r="L2" s="12">
+        <v>3</v>
+      </c>
+      <c r="M2" s="12">
         <v>1</v>
       </c>
-      <c r="F2" s="67">
-        <v>0</v>
-      </c>
-      <c r="G2" s="67">
-        <v>1</v>
-      </c>
-      <c r="H2" s="16">
-        <v>4</v>
-      </c>
-      <c r="I2" s="91">
-        <v>35692</v>
-      </c>
-      <c r="J2" s="12">
-        <v>3</v>
-      </c>
-      <c r="K2" s="12">
-        <v>0</v>
-      </c>
-      <c r="L2" s="12">
-        <v>0</v>
-      </c>
-      <c r="M2" s="12">
-        <v>7</v>
-      </c>
       <c r="N2" s="1" t="s">
-        <v>318</v>
+        <v>380</v>
       </c>
       <c r="O2" t="s">
         <v>412</v>
@@ -15064,46 +15064,46 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="12">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B3" s="103">
-        <v>5</v>
-      </c>
-      <c r="C3" s="21">
+        <v>3</v>
+      </c>
+      <c r="C3" s="64">
         <v>1</v>
       </c>
-      <c r="D3" s="21">
-        <v>1</v>
-      </c>
-      <c r="E3" s="21">
+      <c r="D3" s="64">
+        <v>0</v>
+      </c>
+      <c r="E3" s="64">
+        <v>2</v>
+      </c>
+      <c r="F3" s="20">
+        <v>0</v>
+      </c>
+      <c r="G3" s="64">
+        <v>0</v>
+      </c>
+      <c r="H3" s="16">
+        <v>2</v>
+      </c>
+      <c r="I3" s="91">
+        <v>244318</v>
+      </c>
+      <c r="J3" s="12">
+        <v>21</v>
+      </c>
+      <c r="K3" s="12">
+        <v>0</v>
+      </c>
+      <c r="L3" s="12">
         <v>3</v>
       </c>
-      <c r="F3" s="21">
-        <v>0</v>
-      </c>
-      <c r="G3" s="21">
-        <v>0</v>
-      </c>
-      <c r="H3" s="16">
-        <v>3</v>
-      </c>
-      <c r="I3" s="91">
-        <v>59325</v>
-      </c>
-      <c r="J3" s="12">
-        <v>5</v>
-      </c>
-      <c r="K3" s="12">
-        <v>0</v>
-      </c>
-      <c r="L3" s="12">
-        <v>0</v>
-      </c>
       <c r="M3" s="12">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>318</v>
+        <v>380</v>
       </c>
       <c r="O3" t="s">
         <v>412</v>
@@ -15111,34 +15111,34 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="12">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B4" s="103">
-        <v>5</v>
-      </c>
-      <c r="C4" s="21">
-        <v>0</v>
-      </c>
-      <c r="D4" s="21">
+        <v>3</v>
+      </c>
+      <c r="C4" s="64">
         <v>2</v>
       </c>
-      <c r="E4" s="21">
-        <v>0</v>
-      </c>
-      <c r="F4" s="21">
+      <c r="D4" s="64">
+        <v>0</v>
+      </c>
+      <c r="E4" s="64">
+        <v>0</v>
+      </c>
+      <c r="F4" s="64">
         <v>1</v>
       </c>
-      <c r="G4" s="21">
+      <c r="G4" s="64">
+        <v>0</v>
+      </c>
+      <c r="H4" s="16">
         <v>2</v>
       </c>
-      <c r="H4" s="16">
-        <v>3</v>
-      </c>
       <c r="I4" s="91">
-        <v>47647</v>
+        <v>589620</v>
       </c>
       <c r="J4" s="12">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="K4" s="12">
         <v>0</v>
@@ -15147,51 +15147,51 @@
         <v>2</v>
       </c>
       <c r="M4" s="12">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>318</v>
+        <v>380</v>
       </c>
       <c r="O4" t="s">
         <v>412</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
-        <v>447</v>
+      <c r="A5" s="12">
+        <v>28</v>
       </c>
       <c r="B5" s="103">
-        <v>4</v>
-      </c>
-      <c r="C5" s="21">
+        <v>3</v>
+      </c>
+      <c r="C5" s="68">
+        <v>3</v>
+      </c>
+      <c r="D5" s="68">
+        <v>0</v>
+      </c>
+      <c r="E5" s="68">
+        <v>0</v>
+      </c>
+      <c r="F5" s="68">
+        <v>0</v>
+      </c>
+      <c r="G5" s="68">
+        <v>0</v>
+      </c>
+      <c r="H5" s="16">
         <v>1</v>
       </c>
-      <c r="D5" s="21">
-        <v>0</v>
-      </c>
-      <c r="E5" s="21">
-        <v>0</v>
-      </c>
-      <c r="F5" s="21">
+      <c r="I5" s="91">
+        <v>433721</v>
+      </c>
+      <c r="J5" s="12">
+        <v>36</v>
+      </c>
+      <c r="K5" s="12">
+        <v>0</v>
+      </c>
+      <c r="L5" s="12">
         <v>2</v>
-      </c>
-      <c r="G5" s="21">
-        <v>1</v>
-      </c>
-      <c r="H5" s="16">
-        <v>3</v>
-      </c>
-      <c r="I5" s="91">
-        <v>216523</v>
-      </c>
-      <c r="J5" s="12">
-        <v>18</v>
-      </c>
-      <c r="K5" s="12">
-        <v>0</v>
-      </c>
-      <c r="L5" s="12">
-        <v>3</v>
       </c>
       <c r="M5" s="12">
         <v>1</v>
@@ -15205,182 +15205,182 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="12">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B6" s="103">
         <v>3</v>
       </c>
-      <c r="C6" s="19">
-        <v>0</v>
-      </c>
-      <c r="D6" s="19">
-        <v>3</v>
-      </c>
-      <c r="E6" s="19">
-        <v>0</v>
-      </c>
-      <c r="F6" s="19">
-        <v>0</v>
-      </c>
-      <c r="G6" s="19">
+      <c r="C6" s="64">
+        <v>1</v>
+      </c>
+      <c r="D6" s="64">
+        <v>2</v>
+      </c>
+      <c r="E6" s="64">
+        <v>0</v>
+      </c>
+      <c r="F6" s="64">
+        <v>0</v>
+      </c>
+      <c r="G6" s="64">
         <v>0</v>
       </c>
       <c r="H6" s="16">
+        <v>2</v>
+      </c>
+      <c r="I6" s="91">
+        <v>940438</v>
+      </c>
+      <c r="J6" s="12">
+        <v>79</v>
+      </c>
+      <c r="K6" s="12">
         <v>1</v>
       </c>
-      <c r="I6" s="91">
-        <v>36374</v>
-      </c>
-      <c r="J6" s="12">
-        <v>3</v>
-      </c>
-      <c r="K6" s="12">
-        <v>0</v>
-      </c>
       <c r="L6" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M6" s="12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>318</v>
+        <v>380</v>
       </c>
       <c r="O6" t="s">
         <v>412</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="12" t="s">
-        <v>444</v>
-      </c>
-      <c r="B7" s="103">
+      <c r="A7" s="12">
+        <v>22</v>
+      </c>
+      <c r="B7" s="12">
         <v>3</v>
       </c>
       <c r="C7" s="20">
+        <v>1</v>
+      </c>
+      <c r="D7" s="20">
+        <v>0</v>
+      </c>
+      <c r="E7" s="20">
         <v>2</v>
       </c>
-      <c r="D7" s="20">
-        <v>0</v>
-      </c>
-      <c r="E7" s="20">
-        <v>0</v>
-      </c>
       <c r="F7" s="20">
         <v>0</v>
       </c>
       <c r="G7" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7" s="16">
         <v>2</v>
       </c>
       <c r="I7" s="91">
-        <v>114447</v>
+        <v>535739</v>
       </c>
       <c r="J7" s="12">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="K7" s="12">
         <v>0</v>
       </c>
       <c r="L7" s="12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M7" s="12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>318</v>
+        <v>380</v>
       </c>
       <c r="O7" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="Q7" s="9"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="12">
-        <v>20</v>
-      </c>
-      <c r="B8" s="103">
-        <v>3</v>
-      </c>
-      <c r="C8" s="21">
+        <v>4</v>
+      </c>
+      <c r="B8" s="104">
+        <v>10</v>
+      </c>
+      <c r="C8" s="67">
         <v>1</v>
       </c>
-      <c r="D8" s="21">
+      <c r="D8" s="67">
         <v>1</v>
       </c>
-      <c r="E8" s="21">
-        <v>1</v>
-      </c>
-      <c r="F8" s="21">
-        <v>0</v>
-      </c>
-      <c r="G8" s="21">
+      <c r="E8" s="67">
+        <v>4</v>
+      </c>
+      <c r="F8" s="67">
+        <v>4</v>
+      </c>
+      <c r="G8" s="67">
         <v>0</v>
       </c>
       <c r="H8" s="16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I8" s="91">
-        <v>73125</v>
+        <v>1492437</v>
       </c>
       <c r="J8" s="12">
-        <v>6</v>
+        <v>128</v>
       </c>
       <c r="K8" s="12">
         <v>0</v>
       </c>
       <c r="L8" s="12">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M8" s="12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>318</v>
+        <v>380</v>
       </c>
       <c r="O8" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="12">
-        <v>23</v>
-      </c>
-      <c r="B9" s="103">
-        <v>3</v>
-      </c>
-      <c r="C9" s="64">
-        <v>1</v>
-      </c>
-      <c r="D9" s="64">
-        <v>0</v>
-      </c>
-      <c r="E9" s="64">
+        <v>13</v>
+      </c>
+      <c r="B9" s="104">
+        <v>4</v>
+      </c>
+      <c r="C9" s="20">
         <v>2</v>
       </c>
+      <c r="D9" s="20">
+        <v>0</v>
+      </c>
+      <c r="E9" s="20">
+        <v>0</v>
+      </c>
       <c r="F9" s="20">
-        <v>0</v>
-      </c>
-      <c r="G9" s="64">
+        <v>2</v>
+      </c>
+      <c r="G9" s="20">
         <v>0</v>
       </c>
       <c r="H9" s="16">
         <v>2</v>
       </c>
       <c r="I9" s="91">
-        <v>244318</v>
+        <v>829390</v>
       </c>
       <c r="J9" s="12">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="K9" s="12">
         <v>0</v>
       </c>
       <c r="L9" s="12">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M9" s="12">
         <v>0</v>
@@ -15389,95 +15389,95 @@
         <v>380</v>
       </c>
       <c r="O9" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="12">
-        <v>26</v>
-      </c>
-      <c r="B10" s="103">
-        <v>3</v>
-      </c>
-      <c r="C10" s="64">
-        <v>2</v>
-      </c>
-      <c r="D10" s="64">
-        <v>0</v>
-      </c>
-      <c r="E10" s="64">
-        <v>0</v>
-      </c>
-      <c r="F10" s="64">
+        <v>14</v>
+      </c>
+      <c r="B10" s="104">
+        <v>4</v>
+      </c>
+      <c r="C10" s="19">
+        <v>0</v>
+      </c>
+      <c r="D10" s="19">
+        <v>0</v>
+      </c>
+      <c r="E10" s="19">
+        <v>4</v>
+      </c>
+      <c r="F10" s="19">
+        <v>0</v>
+      </c>
+      <c r="G10" s="19">
+        <v>0</v>
+      </c>
+      <c r="H10" s="16">
         <v>1</v>
       </c>
-      <c r="G10" s="64">
-        <v>0</v>
-      </c>
-      <c r="H10" s="16">
-        <v>2</v>
-      </c>
       <c r="I10" s="91">
-        <v>589620</v>
+        <v>518105</v>
       </c>
       <c r="J10" s="12">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="K10" s="12">
         <v>0</v>
       </c>
       <c r="L10" s="12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M10" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>380</v>
       </c>
       <c r="O10" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11" s="12" t="s">
-        <v>446</v>
+      <c r="A11" s="12">
+        <v>6</v>
       </c>
       <c r="B11" s="103">
+        <v>7</v>
+      </c>
+      <c r="C11" s="67">
         <v>3</v>
       </c>
-      <c r="C11" s="64">
-        <v>0</v>
-      </c>
-      <c r="D11" s="64">
+      <c r="D11" s="67">
         <v>2</v>
       </c>
-      <c r="E11" s="64">
-        <v>0</v>
-      </c>
-      <c r="F11" s="64">
-        <v>0</v>
-      </c>
-      <c r="G11" s="64">
+      <c r="E11" s="67">
         <v>1</v>
       </c>
+      <c r="F11" s="67">
+        <v>0</v>
+      </c>
+      <c r="G11" s="67">
+        <v>1</v>
+      </c>
       <c r="H11" s="16">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I11" s="91">
-        <v>119501</v>
+        <v>35692</v>
       </c>
       <c r="J11" s="12">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="K11" s="12">
         <v>0</v>
       </c>
       <c r="L11" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M11" s="12">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>318</v>
@@ -15488,46 +15488,46 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="12">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="B12" s="103">
+        <v>5</v>
+      </c>
+      <c r="C12" s="21">
+        <v>1</v>
+      </c>
+      <c r="D12" s="21">
+        <v>1</v>
+      </c>
+      <c r="E12" s="21">
         <v>3</v>
       </c>
-      <c r="C12" s="68">
+      <c r="F12" s="21">
+        <v>0</v>
+      </c>
+      <c r="G12" s="21">
+        <v>0</v>
+      </c>
+      <c r="H12" s="16">
         <v>3</v>
       </c>
-      <c r="D12" s="68">
-        <v>0</v>
-      </c>
-      <c r="E12" s="68">
-        <v>0</v>
-      </c>
-      <c r="F12" s="68">
-        <v>0</v>
-      </c>
-      <c r="G12" s="68">
-        <v>0</v>
-      </c>
-      <c r="H12" s="16">
-        <v>1</v>
-      </c>
       <c r="I12" s="91">
-        <v>433721</v>
+        <v>59325</v>
       </c>
       <c r="J12" s="12">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="K12" s="12">
         <v>0</v>
       </c>
       <c r="L12" s="12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M12" s="12">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>380</v>
+        <v>318</v>
       </c>
       <c r="O12" t="s">
         <v>412</v>
@@ -15535,46 +15535,46 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="12">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="B13" s="103">
+        <v>5</v>
+      </c>
+      <c r="C13" s="21">
+        <v>0</v>
+      </c>
+      <c r="D13" s="21">
+        <v>2</v>
+      </c>
+      <c r="E13" s="21">
+        <v>0</v>
+      </c>
+      <c r="F13" s="21">
+        <v>1</v>
+      </c>
+      <c r="G13" s="21">
+        <v>2</v>
+      </c>
+      <c r="H13" s="16">
         <v>3</v>
       </c>
-      <c r="C13" s="64">
-        <v>1</v>
-      </c>
-      <c r="D13" s="64">
-        <v>2</v>
-      </c>
-      <c r="E13" s="64">
-        <v>0</v>
-      </c>
-      <c r="F13" s="64">
-        <v>0</v>
-      </c>
-      <c r="G13" s="64">
-        <v>0</v>
-      </c>
-      <c r="H13" s="16">
-        <v>2</v>
-      </c>
       <c r="I13" s="91">
-        <v>940438</v>
+        <v>47647</v>
       </c>
       <c r="J13" s="12">
-        <v>79</v>
+        <v>4</v>
       </c>
       <c r="K13" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L13" s="12">
         <v>2</v>
       </c>
       <c r="M13" s="12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>380</v>
+        <v>318</v>
       </c>
       <c r="O13" t="s">
         <v>412</v>
@@ -15582,150 +15582,150 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="12">
+        <v>17</v>
+      </c>
+      <c r="B14" s="103">
+        <v>3</v>
+      </c>
+      <c r="C14" s="19">
+        <v>0</v>
+      </c>
+      <c r="D14" s="19">
+        <v>3</v>
+      </c>
+      <c r="E14" s="19">
+        <v>0</v>
+      </c>
+      <c r="F14" s="19">
+        <v>0</v>
+      </c>
+      <c r="G14" s="19">
+        <v>0</v>
+      </c>
+      <c r="H14" s="16">
+        <v>1</v>
+      </c>
+      <c r="I14" s="91">
+        <v>36374</v>
+      </c>
+      <c r="J14" s="12">
+        <v>3</v>
+      </c>
+      <c r="K14" s="12">
+        <v>0</v>
+      </c>
+      <c r="L14" s="12">
+        <v>0</v>
+      </c>
+      <c r="M14" s="12">
+        <v>3</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="O14" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15" s="12" t="s">
+        <v>444</v>
+      </c>
+      <c r="B15" s="103">
+        <v>3</v>
+      </c>
+      <c r="C15" s="20">
         <v>2</v>
       </c>
-      <c r="B14" s="12">
-        <v>17</v>
-      </c>
-      <c r="C14" s="67">
-        <v>3</v>
-      </c>
-      <c r="D14" s="67">
-        <v>0</v>
-      </c>
-      <c r="E14" s="67">
-        <v>2</v>
-      </c>
-      <c r="F14" s="67">
-        <v>11</v>
-      </c>
-      <c r="G14" s="67">
+      <c r="D15" s="20">
+        <v>0</v>
+      </c>
+      <c r="E15" s="20">
+        <v>0</v>
+      </c>
+      <c r="F15" s="20">
+        <v>0</v>
+      </c>
+      <c r="G15" s="20">
         <v>1</v>
-      </c>
-      <c r="H14" s="16">
-        <v>4</v>
-      </c>
-      <c r="I14" s="91">
-        <v>2706500</v>
-      </c>
-      <c r="J14" s="12">
-        <v>229</v>
-      </c>
-      <c r="K14" s="12">
-        <v>14</v>
-      </c>
-      <c r="L14" s="12">
-        <v>3</v>
-      </c>
-      <c r="M14" s="12">
-        <v>0</v>
-      </c>
-      <c r="N14" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="O14" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A15" s="12">
-        <v>18</v>
-      </c>
-      <c r="B15" s="12">
-        <v>3</v>
-      </c>
-      <c r="C15" s="20">
-        <v>0</v>
-      </c>
-      <c r="D15" s="20">
-        <v>2</v>
-      </c>
-      <c r="E15" s="20">
-        <v>1</v>
-      </c>
-      <c r="F15" s="20">
-        <v>0</v>
-      </c>
-      <c r="G15" s="20">
-        <v>0</v>
       </c>
       <c r="H15" s="16">
         <v>2</v>
       </c>
       <c r="I15" s="91">
-        <v>24175</v>
+        <v>114447</v>
       </c>
       <c r="J15" s="12">
+        <v>10</v>
+      </c>
+      <c r="K15" s="12">
+        <v>0</v>
+      </c>
+      <c r="L15" s="12">
+        <v>1</v>
+      </c>
+      <c r="M15" s="12">
         <v>2</v>
-      </c>
-      <c r="K15" s="12">
-        <v>0</v>
-      </c>
-      <c r="L15" s="12">
-        <v>0</v>
-      </c>
-      <c r="M15" s="12">
-        <v>3</v>
       </c>
       <c r="N15" s="1" t="s">
         <v>318</v>
       </c>
       <c r="O15" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="12">
-        <v>22</v>
-      </c>
-      <c r="B16" s="12">
+        <v>20</v>
+      </c>
+      <c r="B16" s="103">
         <v>3</v>
       </c>
-      <c r="C16" s="20">
+      <c r="C16" s="21">
         <v>1</v>
       </c>
-      <c r="D16" s="20">
-        <v>0</v>
-      </c>
-      <c r="E16" s="20">
-        <v>2</v>
-      </c>
-      <c r="F16" s="20">
-        <v>0</v>
-      </c>
-      <c r="G16" s="20">
+      <c r="D16" s="21">
+        <v>1</v>
+      </c>
+      <c r="E16" s="21">
+        <v>1</v>
+      </c>
+      <c r="F16" s="21">
+        <v>0</v>
+      </c>
+      <c r="G16" s="21">
         <v>0</v>
       </c>
       <c r="H16" s="16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I16" s="91">
-        <v>535739</v>
+        <v>73125</v>
       </c>
       <c r="J16" s="12">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="K16" s="12">
         <v>0</v>
       </c>
       <c r="L16" s="12">
+        <v>0</v>
+      </c>
+      <c r="M16" s="12">
         <v>3</v>
       </c>
-      <c r="M16" s="12">
-        <v>0</v>
-      </c>
       <c r="N16" s="1" t="s">
-        <v>380</v>
+        <v>318</v>
       </c>
       <c r="O16" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
     </row>
     <row r="17" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="12">
-        <v>25</v>
-      </c>
-      <c r="B17" s="12">
+      <c r="A17" s="12" t="s">
+        <v>446</v>
+      </c>
+      <c r="B17" s="103">
         <v>3</v>
       </c>
       <c r="C17" s="64">
@@ -15735,117 +15735,117 @@
         <v>2</v>
       </c>
       <c r="E17" s="64">
+        <v>0</v>
+      </c>
+      <c r="F17" s="64">
+        <v>0</v>
+      </c>
+      <c r="G17" s="64">
         <v>1</v>
-      </c>
-      <c r="F17" s="20">
-        <v>0</v>
-      </c>
-      <c r="G17" s="64">
-        <v>0</v>
       </c>
       <c r="H17" s="16">
         <v>2</v>
       </c>
       <c r="I17" s="91">
-        <v>35952</v>
+        <v>119501</v>
       </c>
       <c r="J17" s="12">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="K17" s="12">
         <v>0</v>
       </c>
       <c r="L17" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M17" s="12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N17" s="1" t="s">
         <v>318</v>
       </c>
       <c r="O17" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
     </row>
     <row r="18" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12">
+        <v>18</v>
+      </c>
+      <c r="B18" s="12">
+        <v>3</v>
+      </c>
+      <c r="C18" s="20">
+        <v>0</v>
+      </c>
+      <c r="D18" s="20">
+        <v>2</v>
+      </c>
+      <c r="E18" s="20">
         <v>1</v>
       </c>
-      <c r="B18" s="104">
-        <v>39</v>
-      </c>
-      <c r="C18" s="18">
-        <v>21</v>
-      </c>
-      <c r="D18" s="18">
-        <v>6</v>
-      </c>
-      <c r="E18" s="18">
+      <c r="F18" s="20">
+        <v>0</v>
+      </c>
+      <c r="G18" s="20">
+        <v>0</v>
+      </c>
+      <c r="H18" s="16">
+        <v>2</v>
+      </c>
+      <c r="I18" s="91">
+        <v>24175</v>
+      </c>
+      <c r="J18" s="12">
+        <v>2</v>
+      </c>
+      <c r="K18" s="12">
+        <v>0</v>
+      </c>
+      <c r="L18" s="12">
+        <v>0</v>
+      </c>
+      <c r="M18" s="12">
         <v>3</v>
-      </c>
-      <c r="F18" s="18">
-        <v>5</v>
-      </c>
-      <c r="G18" s="18">
-        <v>4</v>
-      </c>
-      <c r="H18" s="16">
-        <v>5</v>
-      </c>
-      <c r="I18" s="91">
-        <v>280627</v>
-      </c>
-      <c r="J18" s="12">
-        <v>24</v>
-      </c>
-      <c r="K18" s="12">
-        <v>0</v>
-      </c>
-      <c r="L18" s="12">
-        <v>3</v>
-      </c>
-      <c r="M18" s="12">
-        <v>36</v>
       </c>
       <c r="N18" s="1" t="s">
         <v>318</v>
       </c>
       <c r="O18" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="19" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12">
+        <v>25</v>
+      </c>
+      <c r="B19" s="12">
         <v>3</v>
       </c>
-      <c r="B19" s="104">
-        <v>13</v>
-      </c>
-      <c r="C19" s="21">
-        <v>10</v>
-      </c>
-      <c r="D19" s="21">
+      <c r="C19" s="64">
+        <v>0</v>
+      </c>
+      <c r="D19" s="64">
+        <v>2</v>
+      </c>
+      <c r="E19" s="64">
         <v>1</v>
       </c>
-      <c r="E19" s="21">
-        <v>0</v>
-      </c>
-      <c r="F19" s="21">
-        <v>0</v>
-      </c>
-      <c r="G19" s="21">
+      <c r="F19" s="20">
+        <v>0</v>
+      </c>
+      <c r="G19" s="64">
+        <v>0</v>
+      </c>
+      <c r="H19" s="16">
         <v>2</v>
       </c>
-      <c r="H19" s="16">
+      <c r="I19" s="91">
+        <v>35952</v>
+      </c>
+      <c r="J19" s="12">
         <v>3</v>
       </c>
-      <c r="I19" s="91">
-        <v>165633</v>
-      </c>
-      <c r="J19" s="12">
-        <v>14</v>
-      </c>
       <c r="K19" s="12">
         <v>0</v>
       </c>
@@ -15853,57 +15853,57 @@
         <v>0</v>
       </c>
       <c r="M19" s="12">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="N19" s="1" t="s">
         <v>318</v>
       </c>
       <c r="O19" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="12">
+        <v>1</v>
+      </c>
+      <c r="B20" s="104">
+        <v>39</v>
+      </c>
+      <c r="C20" s="18">
+        <v>21</v>
+      </c>
+      <c r="D20" s="18">
+        <v>6</v>
+      </c>
+      <c r="E20" s="18">
+        <v>3</v>
+      </c>
+      <c r="F20" s="18">
+        <v>5</v>
+      </c>
+      <c r="G20" s="18">
         <v>4</v>
       </c>
-      <c r="B20" s="104">
-        <v>10</v>
-      </c>
-      <c r="C20" s="67">
-        <v>1</v>
-      </c>
-      <c r="D20" s="67">
-        <v>1</v>
-      </c>
-      <c r="E20" s="67">
-        <v>4</v>
-      </c>
-      <c r="F20" s="67">
-        <v>4</v>
-      </c>
-      <c r="G20" s="67">
-        <v>0</v>
-      </c>
       <c r="H20" s="16">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I20" s="91">
-        <v>1492437</v>
+        <v>280627</v>
       </c>
       <c r="J20" s="12">
-        <v>128</v>
+        <v>24</v>
       </c>
       <c r="K20" s="12">
         <v>0</v>
       </c>
       <c r="L20" s="12">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="M20" s="12">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>380</v>
+        <v>318</v>
       </c>
       <c r="O20" t="s">
         <v>410</v>
@@ -15911,43 +15911,43 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="12">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B21" s="104">
-        <v>8</v>
-      </c>
-      <c r="C21" s="20">
-        <v>6</v>
-      </c>
-      <c r="D21" s="20">
-        <v>0</v>
-      </c>
-      <c r="E21" s="20">
+        <v>13</v>
+      </c>
+      <c r="C21" s="21">
+        <v>10</v>
+      </c>
+      <c r="D21" s="21">
+        <v>1</v>
+      </c>
+      <c r="E21" s="21">
+        <v>0</v>
+      </c>
+      <c r="F21" s="21">
+        <v>0</v>
+      </c>
+      <c r="G21" s="21">
         <v>2</v>
       </c>
-      <c r="F21" s="20">
-        <v>0</v>
-      </c>
-      <c r="G21" s="20">
-        <v>0</v>
-      </c>
       <c r="H21" s="16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I21" s="91">
-        <v>59753</v>
+        <v>165633</v>
       </c>
       <c r="J21" s="12">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="K21" s="12">
         <v>0</v>
       </c>
       <c r="L21" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M21" s="12">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="N21" s="1" t="s">
         <v>318</v>
@@ -15958,40 +15958,40 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="12">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B22" s="104">
-        <v>7</v>
-      </c>
-      <c r="C22" s="21">
+        <v>8</v>
+      </c>
+      <c r="C22" s="20">
+        <v>6</v>
+      </c>
+      <c r="D22" s="20">
+        <v>0</v>
+      </c>
+      <c r="E22" s="20">
         <v>2</v>
       </c>
-      <c r="D22" s="21">
-        <v>4</v>
-      </c>
-      <c r="E22" s="21">
+      <c r="F22" s="20">
+        <v>0</v>
+      </c>
+      <c r="G22" s="20">
+        <v>0</v>
+      </c>
+      <c r="H22" s="16">
+        <v>2</v>
+      </c>
+      <c r="I22" s="91">
+        <v>59753</v>
+      </c>
+      <c r="J22" s="12">
+        <v>5</v>
+      </c>
+      <c r="K22" s="12">
+        <v>0</v>
+      </c>
+      <c r="L22" s="12">
         <v>1</v>
-      </c>
-      <c r="F22" s="21">
-        <v>0</v>
-      </c>
-      <c r="G22" s="21">
-        <v>0</v>
-      </c>
-      <c r="H22" s="16">
-        <v>3</v>
-      </c>
-      <c r="I22" s="91">
-        <v>35850</v>
-      </c>
-      <c r="J22" s="12">
-        <v>3</v>
-      </c>
-      <c r="K22" s="12">
-        <v>0</v>
-      </c>
-      <c r="L22" s="12">
-        <v>0</v>
       </c>
       <c r="M22" s="12">
         <v>7</v>
@@ -16005,34 +16005,34 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="12">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B23" s="104">
-        <v>6</v>
-      </c>
-      <c r="C23" s="20">
-        <v>5</v>
-      </c>
-      <c r="D23" s="20">
+        <v>7</v>
+      </c>
+      <c r="C23" s="21">
+        <v>2</v>
+      </c>
+      <c r="D23" s="21">
+        <v>4</v>
+      </c>
+      <c r="E23" s="21">
         <v>1</v>
       </c>
-      <c r="E23" s="20">
-        <v>0</v>
-      </c>
-      <c r="F23" s="20">
-        <v>0</v>
-      </c>
-      <c r="G23" s="20">
+      <c r="F23" s="21">
+        <v>0</v>
+      </c>
+      <c r="G23" s="21">
         <v>0</v>
       </c>
       <c r="H23" s="16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I23" s="91">
-        <v>69341</v>
+        <v>35850</v>
       </c>
       <c r="J23" s="12">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="K23" s="12">
         <v>0</v>
@@ -16041,7 +16041,7 @@
         <v>0</v>
       </c>
       <c r="M23" s="12">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N23" s="1" t="s">
         <v>318</v>
@@ -16052,43 +16052,43 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="12">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B24" s="104">
         <v>6</v>
       </c>
-      <c r="C24" s="21">
-        <v>4</v>
-      </c>
-      <c r="D24" s="21">
-        <v>0</v>
-      </c>
-      <c r="E24" s="21">
+      <c r="C24" s="20">
+        <v>5</v>
+      </c>
+      <c r="D24" s="20">
         <v>1</v>
       </c>
-      <c r="F24" s="21">
-        <v>0</v>
-      </c>
-      <c r="G24" s="21">
-        <v>1</v>
+      <c r="E24" s="20">
+        <v>0</v>
+      </c>
+      <c r="F24" s="20">
+        <v>0</v>
+      </c>
+      <c r="G24" s="20">
+        <v>0</v>
       </c>
       <c r="H24" s="16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I24" s="91">
-        <v>201503</v>
+        <v>69341</v>
       </c>
       <c r="J24" s="12">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="K24" s="12">
         <v>0</v>
       </c>
       <c r="L24" s="12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M24" s="12">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="N24" s="1" t="s">
         <v>318</v>
@@ -16099,40 +16099,40 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="12">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B25" s="104">
+        <v>6</v>
+      </c>
+      <c r="C25" s="21">
         <v>4</v>
       </c>
-      <c r="C25" s="20">
+      <c r="D25" s="21">
+        <v>0</v>
+      </c>
+      <c r="E25" s="21">
+        <v>1</v>
+      </c>
+      <c r="F25" s="21">
+        <v>0</v>
+      </c>
+      <c r="G25" s="21">
+        <v>1</v>
+      </c>
+      <c r="H25" s="16">
         <v>3</v>
       </c>
-      <c r="D25" s="20">
-        <v>1</v>
-      </c>
-      <c r="E25" s="20">
-        <v>0</v>
-      </c>
-      <c r="F25" s="20">
-        <v>0</v>
-      </c>
-      <c r="G25" s="20">
-        <v>0</v>
-      </c>
-      <c r="H25" s="16">
+      <c r="I25" s="91">
+        <v>201503</v>
+      </c>
+      <c r="J25" s="12">
+        <v>17</v>
+      </c>
+      <c r="K25" s="12">
+        <v>0</v>
+      </c>
+      <c r="L25" s="12">
         <v>2</v>
-      </c>
-      <c r="I25" s="91">
-        <v>70753</v>
-      </c>
-      <c r="J25" s="12">
-        <v>6</v>
-      </c>
-      <c r="K25" s="12">
-        <v>0</v>
-      </c>
-      <c r="L25" s="12">
-        <v>0</v>
       </c>
       <c r="M25" s="12">
         <v>4</v>
@@ -16146,22 +16146,22 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" s="12">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B26" s="104">
         <v>4</v>
       </c>
       <c r="C26" s="20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D26" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26" s="20">
         <v>0</v>
       </c>
       <c r="F26" s="20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G26" s="20">
         <v>0</v>
@@ -16170,22 +16170,22 @@
         <v>2</v>
       </c>
       <c r="I26" s="91">
-        <v>829390</v>
+        <v>70753</v>
       </c>
       <c r="J26" s="12">
-        <v>71</v>
+        <v>6</v>
       </c>
       <c r="K26" s="12">
         <v>0</v>
       </c>
       <c r="L26" s="12">
+        <v>0</v>
+      </c>
+      <c r="M26" s="12">
         <v>4</v>
       </c>
-      <c r="M26" s="12">
-        <v>0</v>
-      </c>
       <c r="N26" s="1" t="s">
-        <v>380</v>
+        <v>318</v>
       </c>
       <c r="O26" t="s">
         <v>410</v>
@@ -16193,46 +16193,46 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="12">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B27" s="104">
         <v>4</v>
       </c>
-      <c r="C27" s="19">
-        <v>0</v>
-      </c>
-      <c r="D27" s="19">
-        <v>0</v>
-      </c>
-      <c r="E27" s="19">
+      <c r="C27" s="20">
+        <v>1</v>
+      </c>
+      <c r="D27" s="20">
+        <v>3</v>
+      </c>
+      <c r="E27" s="20">
+        <v>0</v>
+      </c>
+      <c r="F27" s="20">
+        <v>0</v>
+      </c>
+      <c r="G27" s="20">
+        <v>0</v>
+      </c>
+      <c r="H27" s="16">
+        <v>2</v>
+      </c>
+      <c r="I27" s="91">
+        <v>131575</v>
+      </c>
+      <c r="J27" s="12">
+        <v>11</v>
+      </c>
+      <c r="K27" s="12">
+        <v>0</v>
+      </c>
+      <c r="L27" s="12">
+        <v>0</v>
+      </c>
+      <c r="M27" s="12">
         <v>4</v>
       </c>
-      <c r="F27" s="19">
-        <v>0</v>
-      </c>
-      <c r="G27" s="19">
-        <v>0</v>
-      </c>
-      <c r="H27" s="16">
-        <v>1</v>
-      </c>
-      <c r="I27" s="91">
-        <v>518105</v>
-      </c>
-      <c r="J27" s="12">
-        <v>45</v>
-      </c>
-      <c r="K27" s="12">
-        <v>0</v>
-      </c>
-      <c r="L27" s="12">
-        <v>4</v>
-      </c>
-      <c r="M27" s="12">
-        <v>0</v>
-      </c>
       <c r="N27" s="1" t="s">
-        <v>380</v>
+        <v>318</v>
       </c>
       <c r="O27" t="s">
         <v>410</v>
@@ -16240,22 +16240,22 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" s="12">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B28" s="104">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C28" s="20">
+        <v>2</v>
+      </c>
+      <c r="D28" s="20">
+        <v>0</v>
+      </c>
+      <c r="E28" s="20">
+        <v>0</v>
+      </c>
+      <c r="F28" s="20">
         <v>1</v>
-      </c>
-      <c r="D28" s="20">
-        <v>3</v>
-      </c>
-      <c r="E28" s="20">
-        <v>0</v>
-      </c>
-      <c r="F28" s="20">
-        <v>0</v>
       </c>
       <c r="G28" s="20">
         <v>0</v>
@@ -16264,7 +16264,7 @@
         <v>2</v>
       </c>
       <c r="I28" s="91">
-        <v>131575</v>
+        <v>128339</v>
       </c>
       <c r="J28" s="12">
         <v>11</v>
@@ -16273,10 +16273,10 @@
         <v>0</v>
       </c>
       <c r="L28" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M28" s="12">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N28" s="1" t="s">
         <v>318</v>
@@ -16286,44 +16286,44 @@
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A29" s="12">
-        <v>21</v>
+      <c r="A29" s="12" t="s">
+        <v>445</v>
       </c>
       <c r="B29" s="104">
         <v>3</v>
       </c>
-      <c r="C29" s="20">
+      <c r="C29" s="64">
         <v>2</v>
       </c>
-      <c r="D29" s="20">
-        <v>0</v>
-      </c>
-      <c r="E29" s="20">
+      <c r="D29" s="64">
+        <v>0</v>
+      </c>
+      <c r="E29" s="64">
         <v>0</v>
       </c>
       <c r="F29" s="20">
+        <v>0</v>
+      </c>
+      <c r="G29" s="64">
         <v>1</v>
-      </c>
-      <c r="G29" s="20">
-        <v>0</v>
       </c>
       <c r="H29" s="16">
         <v>2</v>
       </c>
       <c r="I29" s="91">
-        <v>128339</v>
+        <v>22447</v>
       </c>
       <c r="J29" s="12">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="K29" s="12">
         <v>0</v>
       </c>
       <c r="L29" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M29" s="12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N29" s="1" t="s">
         <v>318</v>
@@ -16333,50 +16333,50 @@
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A30" s="12" t="s">
-        <v>445</v>
-      </c>
-      <c r="B30" s="104">
+      <c r="A30" s="12">
+        <v>2</v>
+      </c>
+      <c r="B30" s="12">
+        <v>17</v>
+      </c>
+      <c r="C30" s="67">
         <v>3</v>
       </c>
-      <c r="C30" s="64">
+      <c r="D30" s="67">
+        <v>0</v>
+      </c>
+      <c r="E30" s="67">
         <v>2</v>
       </c>
-      <c r="D30" s="64">
-        <v>0</v>
-      </c>
-      <c r="E30" s="64">
-        <v>0</v>
-      </c>
-      <c r="F30" s="20">
-        <v>0</v>
-      </c>
-      <c r="G30" s="64">
+      <c r="F30" s="67">
+        <v>11</v>
+      </c>
+      <c r="G30" s="67">
         <v>1</v>
       </c>
       <c r="H30" s="16">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I30" s="91">
-        <v>22447</v>
+        <v>2706500</v>
       </c>
       <c r="J30" s="12">
-        <v>2</v>
+        <v>229</v>
       </c>
       <c r="K30" s="12">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="L30" s="12">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M30" s="12">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="O30" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.2">
@@ -16403,7 +16403,7 @@
   </sheetData>
   <autoFilter ref="A1:O23" xr:uid="{DE1A20C9-41D8-6D4F-99AC-E85332934F3C}">
     <sortState ref="A2:O30">
-      <sortCondition ref="O1:O30"/>
+      <sortCondition ref="N1:N30"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16414,7 +16414,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD78233B-E478-774A-8E5D-0A41164AE470}">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -17580,7 +17580,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19A69BF1-CCFD-6443-93E0-6139599E6807}">
   <dimension ref="A1:P42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
@@ -17598,7 +17598,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="J1" s="123" t="s">
+      <c r="J1" s="117" t="s">
         <v>450</v>
       </c>
     </row>
@@ -18200,15 +18200,15 @@
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A18" s="121" t="s">
+      <c r="A18" s="122" t="s">
         <v>399</v>
       </c>
-      <c r="B18" s="121"/>
-      <c r="C18" s="121"/>
-      <c r="D18" s="121"/>
-      <c r="E18" s="121"/>
-      <c r="F18" s="121"/>
-      <c r="G18" s="121"/>
+      <c r="B18" s="122"/>
+      <c r="C18" s="122"/>
+      <c r="D18" s="122"/>
+      <c r="E18" s="122"/>
+      <c r="F18" s="122"/>
+      <c r="G18" s="122"/>
       <c r="I18" s="73"/>
       <c r="L18">
         <f>9/13</f>
@@ -18418,15 +18418,15 @@
       <c r="G26" s="8"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A27" s="122" t="s">
+      <c r="A27" s="123" t="s">
         <v>324</v>
       </c>
-      <c r="B27" s="122"/>
-      <c r="C27" s="122"/>
-      <c r="D27" s="122"/>
-      <c r="E27" s="122"/>
-      <c r="F27" s="122"/>
-      <c r="G27" s="122"/>
+      <c r="B27" s="123"/>
+      <c r="C27" s="123"/>
+      <c r="D27" s="123"/>
+      <c r="E27" s="123"/>
+      <c r="F27" s="123"/>
+      <c r="G27" s="123"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="102"/>

</xml_diff>